<commit_message>
Removal of the IOTC main area from the stratum of the 2 FC form
</commit_message>
<xml_diff>
--- a/form_reporting_templates/Form-2FC.xlsx
+++ b/form_reporting_templates/Form-2FC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\dev\git\BitBucket workspaces\IOTC-ws\Data dissemination\iotc-reference-forms\form_reporting_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\iotc-reference-forms\form_reporting_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4F88A2-31D2-490E-90C5-CC2D24FD4E5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1045DC96-AB39-457F-AEF5-97A7DBFAB79F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="wX8sA2MiVV4hem5/4RTiTmcDJYFB86HqbOVJt9hNWIZw6gEt8u041CW+Lo33VdE+XPx62lk39pDAbSFn1bENfA==" workbookSaltValue="4+KZsXogYyQ9Ht7v5WkMIg==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>Focal point</t>
   </si>
@@ -114,9 +114,6 @@
     <t>%</t>
   </si>
   <si>
-    <t>IOTC area</t>
-  </si>
-  <si>
     <t>Reporting entity</t>
   </si>
   <si>
@@ -147,10 +144,10 @@
     <t>Flag state</t>
   </si>
   <si>
-    <t>Main elements</t>
-  </si>
-  <si>
     <t>Storage</t>
+  </si>
+  <si>
+    <t>Main element</t>
   </si>
 </sst>
 </file>
@@ -626,7 +623,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -810,6 +807,9 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1208,24 +1208,24 @@
   <sheetData>
     <row r="1" spans="2:8" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="67" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="69"/>
+      <c r="B2" s="68" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="70"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="70"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="72"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="73"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="13"/>
@@ -1233,14 +1233,14 @@
         <v>10</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E4" s="16"/>
       <c r="F4" s="14" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H4" s="18"/>
     </row>
@@ -1275,15 +1275,15 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="19"/>
-      <c r="C8" s="66" t="s">
+      <c r="C8" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="66"/>
+      <c r="D8" s="67"/>
       <c r="E8" s="20"/>
-      <c r="F8" s="66" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" s="66"/>
+      <c r="F8" s="67" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="67"/>
       <c r="H8" s="21"/>
     </row>
     <row r="9" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1302,12 +1302,12 @@
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="19"/>
       <c r="C10" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="20"/>
       <c r="F10" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="21"/>
@@ -1324,7 +1324,7 @@
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="19"/>
       <c r="C12" s="24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12" s="40"/>
       <c r="E12" s="20"/>
@@ -1395,7 +1395,7 @@
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="19"/>
       <c r="C19" s="41" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="20"/>
@@ -1406,7 +1406,7 @@
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="19"/>
       <c r="C20" s="42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="20"/>
@@ -1454,11 +1454,11 @@
     </row>
     <row r="25" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="19"/>
-      <c r="C25" s="63"/>
-      <c r="D25" s="64"/>
-      <c r="E25" s="64"/>
-      <c r="F25" s="64"/>
-      <c r="G25" s="65"/>
+      <c r="C25" s="64"/>
+      <c r="D25" s="65"/>
+      <c r="E25" s="65"/>
+      <c r="F25" s="65"/>
+      <c r="G25" s="66"/>
       <c r="H25" s="21"/>
     </row>
     <row r="26" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1498,7 +1498,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:P55"/>
+  <dimension ref="A1:O55"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
@@ -1511,23 +1511,22 @@
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" style="38" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="39" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="38" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="43" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="39" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="38" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="46" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="38"/>
-    <col min="10" max="10" width="14.28515625" style="39" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" style="38" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" style="39" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="38"/>
-    <col min="14" max="14" width="9.140625" style="49"/>
-    <col min="15" max="15" width="9.140625" style="50"/>
-    <col min="16" max="16" width="9.140625" style="52"/>
+    <col min="3" max="3" width="11.42578125" style="38" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="43" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="39" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="38" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="46" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="38"/>
+    <col min="9" max="9" width="14.28515625" style="39" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" style="38" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="39" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="38"/>
+    <col min="13" max="13" width="9.140625" style="49"/>
+    <col min="14" max="14" width="9.140625" style="50"/>
+    <col min="15" max="15" width="9.140625" style="52"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1"/>
@@ -1541,866 +1540,804 @@
       <c r="L1"/>
       <c r="M1"/>
       <c r="N1"/>
-      <c r="O1"/>
-      <c r="P1" s="8"/>
-    </row>
-    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="67" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="68"/>
-      <c r="L2" s="68"/>
-      <c r="M2" s="68"/>
-      <c r="N2" s="68"/>
-      <c r="O2" s="68"/>
-      <c r="P2" s="69"/>
-    </row>
-    <row r="3" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O1" s="8"/>
+    </row>
+    <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="68" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="69"/>
+      <c r="M2" s="69"/>
+      <c r="N2" s="69"/>
+      <c r="O2" s="70"/>
+    </row>
+    <row r="3" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
-      <c r="B3" s="70"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="71"/>
-      <c r="O3" s="71"/>
-      <c r="P3" s="72"/>
-    </row>
-    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="71"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="72"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="72"/>
+      <c r="O3" s="73"/>
+    </row>
+    <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
-      <c r="B4" s="73" t="s">
+      <c r="B4" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="75"/>
-      <c r="D4" s="73" t="s">
+      <c r="C4" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="74"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="73" t="s">
+      <c r="D4" s="75"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="75"/>
-      <c r="I4" s="73" t="s">
+      <c r="G4" s="76"/>
+      <c r="H4" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="75"/>
-      <c r="K4" s="73" t="s">
+      <c r="I4" s="76"/>
+      <c r="J4" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="75"/>
-      <c r="M4" s="73" t="s">
+      <c r="K4" s="76"/>
+      <c r="L4" s="74" t="s">
         <v>19</v>
       </c>
-      <c r="N4" s="74"/>
-      <c r="O4" s="75"/>
-      <c r="P4" s="33" t="s">
+      <c r="M4" s="75"/>
+      <c r="N4" s="76"/>
+      <c r="O4" s="33" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="56" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="57" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="62" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="58" t="s">
+      <c r="D5" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="59" t="s">
+      <c r="E5" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="53" t="s">
+      <c r="F5" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="54" t="s">
+      <c r="G5" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="56" t="s">
+      <c r="H5" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="57" t="s">
+      <c r="I5" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="56" t="s">
+      <c r="J5" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="57" t="s">
-        <v>37</v>
-      </c>
-      <c r="M5" s="56" t="s">
+      <c r="K5" s="57" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="N5" s="60" t="s">
+      <c r="M5" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="O5" s="61" t="s">
+      <c r="N5" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="P5" s="55" t="s">
+      <c r="O5" s="55" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B6" s="10"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="34"/>
-      <c r="L6" s="35"/>
-      <c r="M6" s="34"/>
-      <c r="N6" s="47"/>
-      <c r="O6" s="48"/>
-      <c r="P6" s="51"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C6" s="10"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="48"/>
+      <c r="O6" s="51"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="36"/>
-      <c r="L7" s="37"/>
-      <c r="M7" s="36"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C7" s="5"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="36"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="36"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="36"/>
-      <c r="L8" s="37"/>
-      <c r="M8" s="36"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C8" s="5"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="36"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="36"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="37"/>
-      <c r="M9" s="36"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C9" s="5"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="36"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="37"/>
-      <c r="K10" s="36"/>
-      <c r="L10" s="37"/>
-      <c r="M10" s="36"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C10" s="5"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="36"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="36"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="37"/>
-      <c r="K11" s="36"/>
-      <c r="L11" s="37"/>
-      <c r="M11" s="36"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C11" s="5"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="37"/>
+      <c r="L11" s="36"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="45"/>
-      <c r="I12" s="36"/>
-      <c r="J12" s="37"/>
-      <c r="K12" s="36"/>
-      <c r="L12" s="37"/>
-      <c r="M12" s="36"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C12" s="5"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="36"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="36"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="45"/>
-      <c r="I13" s="36"/>
-      <c r="J13" s="37"/>
-      <c r="K13" s="36"/>
-      <c r="L13" s="37"/>
-      <c r="M13" s="36"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C13" s="5"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="36"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="45"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="37"/>
-      <c r="K14" s="36"/>
-      <c r="L14" s="37"/>
-      <c r="M14" s="36"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C14" s="5"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="36"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="36"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="36"/>
-      <c r="J15" s="37"/>
-      <c r="K15" s="36"/>
-      <c r="L15" s="37"/>
-      <c r="M15" s="36"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C15" s="5"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="36"/>
+      <c r="K15" s="37"/>
+      <c r="L15" s="36"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B16" s="5"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="45"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="37"/>
-      <c r="K16" s="36"/>
-      <c r="L16" s="37"/>
-      <c r="M16" s="36"/>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C16" s="5"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="36"/>
+      <c r="K16" s="37"/>
+      <c r="L16" s="36"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="5"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="36"/>
-      <c r="J17" s="37"/>
-      <c r="K17" s="36"/>
-      <c r="L17" s="37"/>
-      <c r="M17" s="36"/>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C17" s="5"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="36"/>
+      <c r="K17" s="37"/>
+      <c r="L17" s="36"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="5"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="45"/>
-      <c r="I18" s="36"/>
-      <c r="J18" s="37"/>
-      <c r="K18" s="36"/>
-      <c r="L18" s="37"/>
-      <c r="M18" s="36"/>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C18" s="5"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="36"/>
+      <c r="K18" s="37"/>
+      <c r="L18" s="36"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="45"/>
-      <c r="I19" s="36"/>
-      <c r="J19" s="37"/>
-      <c r="K19" s="36"/>
-      <c r="L19" s="37"/>
-      <c r="M19" s="36"/>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C19" s="5"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="36"/>
+      <c r="K19" s="37"/>
+      <c r="L19" s="36"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="45"/>
-      <c r="I20" s="36"/>
-      <c r="J20" s="37"/>
-      <c r="K20" s="36"/>
-      <c r="L20" s="37"/>
-      <c r="M20" s="36"/>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C20" s="5"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="45"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="36"/>
+      <c r="K20" s="37"/>
+      <c r="L20" s="36"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="45"/>
-      <c r="I21" s="36"/>
-      <c r="J21" s="37"/>
-      <c r="K21" s="36"/>
-      <c r="L21" s="37"/>
-      <c r="M21" s="36"/>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C21" s="5"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="37"/>
+      <c r="L21" s="36"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" s="5"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="45"/>
-      <c r="I22" s="36"/>
-      <c r="J22" s="37"/>
-      <c r="K22" s="36"/>
-      <c r="L22" s="37"/>
-      <c r="M22" s="36"/>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C22" s="5"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="36"/>
+      <c r="K22" s="37"/>
+      <c r="L22" s="36"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="36"/>
-      <c r="J23" s="37"/>
-      <c r="K23" s="36"/>
-      <c r="L23" s="37"/>
-      <c r="M23" s="36"/>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C23" s="5"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="36"/>
+      <c r="K23" s="37"/>
+      <c r="L23" s="36"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="45"/>
-      <c r="I24" s="36"/>
-      <c r="J24" s="37"/>
-      <c r="K24" s="36"/>
-      <c r="L24" s="37"/>
-      <c r="M24" s="36"/>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C24" s="5"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="37"/>
+      <c r="J24" s="36"/>
+      <c r="K24" s="37"/>
+      <c r="L24" s="36"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="5"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="45"/>
-      <c r="I25" s="36"/>
-      <c r="J25" s="37"/>
-      <c r="K25" s="36"/>
-      <c r="L25" s="37"/>
-      <c r="M25" s="36"/>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C25" s="5"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="45"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="36"/>
+      <c r="K25" s="37"/>
+      <c r="L25" s="36"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="45"/>
-      <c r="I26" s="36"/>
-      <c r="J26" s="37"/>
-      <c r="K26" s="36"/>
-      <c r="L26" s="37"/>
-      <c r="M26" s="36"/>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C26" s="5"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="45"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="36"/>
+      <c r="K26" s="37"/>
+      <c r="L26" s="36"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="45"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="37"/>
-      <c r="K27" s="36"/>
-      <c r="L27" s="37"/>
-      <c r="M27" s="36"/>
-    </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C27" s="5"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="45"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="36"/>
+      <c r="K27" s="37"/>
+      <c r="L27" s="36"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" s="5"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="37"/>
-      <c r="K28" s="36"/>
-      <c r="L28" s="37"/>
-      <c r="M28" s="36"/>
-    </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C28" s="5"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="36"/>
+      <c r="K28" s="37"/>
+      <c r="L28" s="36"/>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="36"/>
-      <c r="J29" s="37"/>
-      <c r="K29" s="36"/>
-      <c r="L29" s="37"/>
-      <c r="M29" s="36"/>
-    </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C29" s="5"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="36"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="36"/>
+      <c r="K29" s="37"/>
+      <c r="L29" s="36"/>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" s="5"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="36"/>
-      <c r="J30" s="37"/>
-      <c r="K30" s="36"/>
-      <c r="L30" s="37"/>
-      <c r="M30" s="36"/>
-    </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C30" s="5"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="37"/>
+      <c r="J30" s="36"/>
+      <c r="K30" s="37"/>
+      <c r="L30" s="36"/>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B31" s="5"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="45"/>
-      <c r="I31" s="36"/>
-      <c r="J31" s="37"/>
-      <c r="K31" s="36"/>
-      <c r="L31" s="37"/>
-      <c r="M31" s="36"/>
-    </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C31" s="5"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="36"/>
+      <c r="I31" s="37"/>
+      <c r="J31" s="36"/>
+      <c r="K31" s="37"/>
+      <c r="L31" s="36"/>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B32" s="5"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="45"/>
-      <c r="I32" s="36"/>
-      <c r="J32" s="37"/>
-      <c r="K32" s="36"/>
-      <c r="L32" s="37"/>
-      <c r="M32" s="36"/>
-    </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C32" s="5"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="45"/>
+      <c r="H32" s="36"/>
+      <c r="I32" s="37"/>
+      <c r="J32" s="36"/>
+      <c r="K32" s="37"/>
+      <c r="L32" s="36"/>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B33" s="5"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="45"/>
-      <c r="I33" s="36"/>
-      <c r="J33" s="37"/>
-      <c r="K33" s="36"/>
-      <c r="L33" s="37"/>
-      <c r="M33" s="36"/>
-    </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C33" s="5"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="45"/>
+      <c r="H33" s="36"/>
+      <c r="I33" s="37"/>
+      <c r="J33" s="36"/>
+      <c r="K33" s="37"/>
+      <c r="L33" s="36"/>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B34" s="5"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="45"/>
-      <c r="I34" s="36"/>
-      <c r="J34" s="37"/>
-      <c r="K34" s="36"/>
-      <c r="L34" s="37"/>
-      <c r="M34" s="36"/>
-    </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C34" s="5"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="45"/>
+      <c r="H34" s="36"/>
+      <c r="I34" s="37"/>
+      <c r="J34" s="36"/>
+      <c r="K34" s="37"/>
+      <c r="L34" s="36"/>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B35" s="5"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="45"/>
-      <c r="I35" s="36"/>
-      <c r="J35" s="37"/>
-      <c r="K35" s="36"/>
-      <c r="L35" s="37"/>
-      <c r="M35" s="36"/>
-    </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C35" s="5"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="45"/>
+      <c r="H35" s="36"/>
+      <c r="I35" s="37"/>
+      <c r="J35" s="36"/>
+      <c r="K35" s="37"/>
+      <c r="L35" s="36"/>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B36" s="5"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="45"/>
-      <c r="I36" s="36"/>
-      <c r="J36" s="37"/>
-      <c r="K36" s="36"/>
-      <c r="L36" s="37"/>
-      <c r="M36" s="36"/>
-    </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C36" s="5"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="45"/>
+      <c r="H36" s="36"/>
+      <c r="I36" s="37"/>
+      <c r="J36" s="36"/>
+      <c r="K36" s="37"/>
+      <c r="L36" s="36"/>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B37" s="5"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="45"/>
-      <c r="I37" s="36"/>
-      <c r="J37" s="37"/>
-      <c r="K37" s="36"/>
-      <c r="L37" s="37"/>
-      <c r="M37" s="36"/>
-    </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C37" s="5"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="45"/>
+      <c r="H37" s="36"/>
+      <c r="I37" s="37"/>
+      <c r="J37" s="36"/>
+      <c r="K37" s="37"/>
+      <c r="L37" s="36"/>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B38" s="5"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="45"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="37"/>
-      <c r="K38" s="36"/>
-      <c r="L38" s="37"/>
-      <c r="M38" s="36"/>
-    </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C38" s="5"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="45"/>
+      <c r="H38" s="36"/>
+      <c r="I38" s="37"/>
+      <c r="J38" s="36"/>
+      <c r="K38" s="37"/>
+      <c r="L38" s="36"/>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B39" s="5"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="5"/>
-      <c r="H39" s="45"/>
-      <c r="I39" s="36"/>
-      <c r="J39" s="37"/>
-      <c r="K39" s="36"/>
-      <c r="L39" s="37"/>
-      <c r="M39" s="36"/>
-    </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C39" s="5"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="45"/>
+      <c r="H39" s="36"/>
+      <c r="I39" s="37"/>
+      <c r="J39" s="36"/>
+      <c r="K39" s="37"/>
+      <c r="L39" s="36"/>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B40" s="5"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="5"/>
-      <c r="H40" s="45"/>
-      <c r="I40" s="36"/>
-      <c r="J40" s="37"/>
-      <c r="K40" s="36"/>
-      <c r="L40" s="37"/>
-      <c r="M40" s="36"/>
-    </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C40" s="5"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="45"/>
+      <c r="H40" s="36"/>
+      <c r="I40" s="37"/>
+      <c r="J40" s="36"/>
+      <c r="K40" s="37"/>
+      <c r="L40" s="36"/>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B41" s="5"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="45"/>
-      <c r="I41" s="36"/>
-      <c r="J41" s="37"/>
-      <c r="K41" s="36"/>
-      <c r="L41" s="37"/>
-      <c r="M41" s="36"/>
-    </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C41" s="5"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="45"/>
+      <c r="H41" s="36"/>
+      <c r="I41" s="37"/>
+      <c r="J41" s="36"/>
+      <c r="K41" s="37"/>
+      <c r="L41" s="36"/>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B42" s="5"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="5"/>
-      <c r="H42" s="45"/>
-      <c r="I42" s="36"/>
-      <c r="J42" s="37"/>
-      <c r="K42" s="36"/>
-      <c r="L42" s="37"/>
-      <c r="M42" s="36"/>
-    </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C42" s="5"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="45"/>
+      <c r="H42" s="36"/>
+      <c r="I42" s="37"/>
+      <c r="J42" s="36"/>
+      <c r="K42" s="37"/>
+      <c r="L42" s="36"/>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B43" s="5"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="5"/>
-      <c r="H43" s="45"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="37"/>
-      <c r="K43" s="36"/>
-      <c r="L43" s="37"/>
-      <c r="M43" s="36"/>
-    </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C43" s="5"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="45"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="37"/>
+      <c r="J43" s="36"/>
+      <c r="K43" s="37"/>
+      <c r="L43" s="36"/>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B44" s="5"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="5"/>
-      <c r="H44" s="45"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="37"/>
-      <c r="K44" s="36"/>
-      <c r="L44" s="37"/>
-      <c r="M44" s="36"/>
-    </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C44" s="5"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="45"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="37"/>
+      <c r="J44" s="36"/>
+      <c r="K44" s="37"/>
+      <c r="L44" s="36"/>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B45" s="5"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="5"/>
-      <c r="H45" s="45"/>
-      <c r="I45" s="36"/>
-      <c r="J45" s="37"/>
-      <c r="K45" s="36"/>
-      <c r="L45" s="37"/>
-      <c r="M45" s="36"/>
-    </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C45" s="5"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="45"/>
+      <c r="H45" s="36"/>
+      <c r="I45" s="37"/>
+      <c r="J45" s="36"/>
+      <c r="K45" s="37"/>
+      <c r="L45" s="36"/>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B46" s="5"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="5"/>
-      <c r="H46" s="45"/>
-      <c r="I46" s="36"/>
-      <c r="J46" s="37"/>
-      <c r="K46" s="36"/>
-      <c r="L46" s="37"/>
-      <c r="M46" s="36"/>
-    </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C46" s="5"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="45"/>
+      <c r="H46" s="36"/>
+      <c r="I46" s="37"/>
+      <c r="J46" s="36"/>
+      <c r="K46" s="37"/>
+      <c r="L46" s="36"/>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B47" s="5"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="7"/>
-      <c r="G47" s="5"/>
-      <c r="H47" s="45"/>
-      <c r="I47" s="36"/>
-      <c r="J47" s="37"/>
-      <c r="K47" s="36"/>
-      <c r="L47" s="37"/>
-      <c r="M47" s="36"/>
-    </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C47" s="5"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="45"/>
+      <c r="H47" s="36"/>
+      <c r="I47" s="37"/>
+      <c r="J47" s="36"/>
+      <c r="K47" s="37"/>
+      <c r="L47" s="36"/>
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B48" s="5"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="7"/>
-      <c r="G48" s="5"/>
-      <c r="H48" s="45"/>
-      <c r="I48" s="36"/>
-      <c r="J48" s="37"/>
-      <c r="K48" s="36"/>
-      <c r="L48" s="37"/>
-      <c r="M48" s="36"/>
-    </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C48" s="5"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="45"/>
+      <c r="H48" s="36"/>
+      <c r="I48" s="37"/>
+      <c r="J48" s="36"/>
+      <c r="K48" s="37"/>
+      <c r="L48" s="36"/>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B49" s="5"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="7"/>
-      <c r="G49" s="5"/>
-      <c r="H49" s="45"/>
-      <c r="I49" s="36"/>
-      <c r="J49" s="37"/>
-      <c r="K49" s="36"/>
-      <c r="L49" s="37"/>
-      <c r="M49" s="36"/>
-    </row>
-    <row r="50" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C49" s="5"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="45"/>
+      <c r="H49" s="36"/>
+      <c r="I49" s="37"/>
+      <c r="J49" s="36"/>
+      <c r="K49" s="37"/>
+      <c r="L49" s="36"/>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B50" s="5"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="7"/>
-      <c r="G50" s="5"/>
-      <c r="H50" s="45"/>
-      <c r="I50" s="36"/>
-      <c r="J50" s="37"/>
-      <c r="K50" s="36"/>
-      <c r="L50" s="37"/>
-      <c r="M50" s="36"/>
-    </row>
-    <row r="51" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C50" s="5"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="45"/>
+      <c r="H50" s="36"/>
+      <c r="I50" s="37"/>
+      <c r="J50" s="36"/>
+      <c r="K50" s="37"/>
+      <c r="L50" s="36"/>
+    </row>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B51" s="5"/>
-      <c r="C51" s="7"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="7"/>
-      <c r="G51" s="5"/>
-      <c r="H51" s="45"/>
-      <c r="I51" s="36"/>
-      <c r="J51" s="37"/>
-      <c r="K51" s="36"/>
-      <c r="L51" s="37"/>
-      <c r="M51" s="36"/>
-    </row>
-    <row r="52" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C51" s="5"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="45"/>
+      <c r="H51" s="36"/>
+      <c r="I51" s="37"/>
+      <c r="J51" s="36"/>
+      <c r="K51" s="37"/>
+      <c r="L51" s="36"/>
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B52" s="5"/>
-      <c r="C52" s="7"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="7"/>
-      <c r="G52" s="5"/>
-      <c r="H52" s="45"/>
-      <c r="I52" s="36"/>
-      <c r="J52" s="37"/>
-      <c r="K52" s="36"/>
-      <c r="L52" s="37"/>
-      <c r="M52" s="36"/>
-    </row>
-    <row r="53" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C52" s="5"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="45"/>
+      <c r="H52" s="36"/>
+      <c r="I52" s="37"/>
+      <c r="J52" s="36"/>
+      <c r="K52" s="37"/>
+      <c r="L52" s="36"/>
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B53" s="5"/>
-      <c r="C53" s="7"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="6"/>
-      <c r="F53" s="7"/>
-      <c r="G53" s="5"/>
-      <c r="H53" s="45"/>
-      <c r="I53" s="36"/>
-      <c r="J53" s="37"/>
-      <c r="K53" s="36"/>
-      <c r="L53" s="37"/>
-      <c r="M53" s="36"/>
-    </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C53" s="5"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="45"/>
+      <c r="H53" s="36"/>
+      <c r="I53" s="37"/>
+      <c r="J53" s="36"/>
+      <c r="K53" s="37"/>
+      <c r="L53" s="36"/>
+    </row>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B54" s="5"/>
-      <c r="C54" s="7"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="6"/>
-      <c r="F54" s="7"/>
-      <c r="G54" s="5"/>
-      <c r="H54" s="45"/>
-      <c r="I54" s="36"/>
-      <c r="J54" s="37"/>
-      <c r="K54" s="36"/>
-      <c r="L54" s="37"/>
-      <c r="M54" s="36"/>
-    </row>
-    <row r="55" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C54" s="5"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="45"/>
+      <c r="H54" s="36"/>
+      <c r="I54" s="37"/>
+      <c r="J54" s="36"/>
+      <c r="K54" s="37"/>
+      <c r="L54" s="36"/>
+    </row>
+    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B55" s="5"/>
-      <c r="C55" s="7"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="6"/>
-      <c r="F55" s="7"/>
-      <c r="G55" s="5"/>
-      <c r="H55" s="45"/>
-      <c r="I55" s="36"/>
-      <c r="J55" s="37"/>
-      <c r="K55" s="36"/>
-      <c r="L55" s="37"/>
-      <c r="M55" s="36"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="45"/>
+      <c r="H55" s="36"/>
+      <c r="I55" s="37"/>
+      <c r="J55" s="36"/>
+      <c r="K55" s="37"/>
+      <c r="L55" s="36"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="9wm5KxQBvaSoGcVWZhpcZByP5kKefPRqeb3RJ/rGLtAXHyBbbNqqPlLgHHjcYlVBA/O8zFg+fZsVipAvIIFQiQ==" saltValue="fQTx0oBU3rfh33Gh5MtEIQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
-  <mergeCells count="7">
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B2:P3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="M4:O4"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="4/x7C4c4a0AVjOBj6btm9hOkWI9rn64Xb2MGYaWzP1gOCmRzIyayQx4ap4mNv9s4uluXIm2VuMoUCNU9Zv82wg==" saltValue="9FPR1JcRdNMeuwdMyreDEw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <mergeCells count="6">
+    <mergeCell ref="B2:O3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:N4"/>
   </mergeCells>
-  <conditionalFormatting sqref="B6:P1048576">
+  <conditionalFormatting sqref="B6:O1048576">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>B6=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:G5 I5:K5 M5" xr:uid="{62AC337C-43B8-43CC-ABCC-7EE87C42A16F}">
-      <formula1>"&lt;0&gt;0"</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5" xr:uid="{FC838703-B75A-43B5-B023-13160A0C8CB9}">
+  <dataValidations count="1">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:L5 B5:F5" xr:uid="{62AC337C-43B8-43CC-ABCC-7EE87C42A16F}">
       <formula1>"&lt;0&gt;0"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1" location="IOTCareasMain" xr:uid="{51E5C891-8AF9-4A30-9A9C-D3EF2615C20A}"/>
-    <hyperlink ref="D5" r:id="rId2" location="types" xr:uid="{37DC6134-83EB-4EAA-AE13-E456A3F41FF0}"/>
-    <hyperlink ref="E5" r:id="rId3" location="sourcesFC" xr:uid="{D508B0C5-71F1-4418-BA5D-6D532A3A0D47}"/>
-    <hyperlink ref="F5" r:id="rId4" location="processingsFC" xr:uid="{3B28F9E8-FD32-4256-82C2-97BF03FEE964}"/>
-    <hyperlink ref="G5" r:id="rId5" location="coverageTypes" xr:uid="{15A256B6-6B98-4ABF-81CC-D96AC29A08E2}"/>
-    <hyperlink ref="I5" r:id="rId6" location="boatTypes" xr:uid="{DADB17F2-537E-4DBC-AFEA-6EE304F8C6D0}"/>
-    <hyperlink ref="J5" r:id="rId7" location="mechanizationTypes" xr:uid="{40C3FFA1-CD46-4638-8E84-B19E43E165D4}"/>
-    <hyperlink ref="K5" r:id="rId8" location="fishPreservationMethods" xr:uid="{2A56DBD0-E939-42A6-98DA-87DA852FD2E9}"/>
-    <hyperlink ref="L5" r:id="rId9" location="fishStorageTypes" xr:uid="{9C5A0F26-DE48-4B7A-BF87-82196056DE69}"/>
-    <hyperlink ref="M5" r:id="rId10" location="boatClassTypes" xr:uid="{263265AE-A782-4C7E-A95B-56C7C8AA2144}"/>
-    <hyperlink ref="B5" r:id="rId11" location="fisheries" xr:uid="{9C9CCABD-E884-4981-9553-0A805CCD876C}"/>
+    <hyperlink ref="C5" r:id="rId1" location="types" xr:uid="{37DC6134-83EB-4EAA-AE13-E456A3F41FF0}"/>
+    <hyperlink ref="D5" r:id="rId2" location="sourcesFC" xr:uid="{D508B0C5-71F1-4418-BA5D-6D532A3A0D47}"/>
+    <hyperlink ref="E5" r:id="rId3" location="processingsFC" xr:uid="{3B28F9E8-FD32-4256-82C2-97BF03FEE964}"/>
+    <hyperlink ref="F5" r:id="rId4" location="coverageTypes" xr:uid="{15A256B6-6B98-4ABF-81CC-D96AC29A08E2}"/>
+    <hyperlink ref="H5" r:id="rId5" location="boatTypes" xr:uid="{DADB17F2-537E-4DBC-AFEA-6EE304F8C6D0}"/>
+    <hyperlink ref="I5" r:id="rId6" location="mechanizationTypes" xr:uid="{40C3FFA1-CD46-4638-8E84-B19E43E165D4}"/>
+    <hyperlink ref="J5" r:id="rId7" location="fishPreservationMethods" xr:uid="{2A56DBD0-E939-42A6-98DA-87DA852FD2E9}"/>
+    <hyperlink ref="K5" r:id="rId8" location="fishStorageTypes" xr:uid="{9C5A0F26-DE48-4B7A-BF87-82196056DE69}"/>
+    <hyperlink ref="L5" r:id="rId9" location="boatClassTypes" xr:uid="{263265AE-A782-4C7E-A95B-56C7C8AA2144}"/>
+    <hyperlink ref="B5" r:id="rId10" location="fisheries" xr:uid="{9C9CCABD-E884-4981-9553-0A805CCD876C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Edits in the description of the form 2FC following feedback from the Data Reporting Workshop
</commit_message>
<xml_diff>
--- a/form_reporting_templates/Form-2FC.xlsx
+++ b/form_reporting_templates/Form-2FC.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\iotc-reference-forms\form_reporting_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\repositories\data-reporting\iotc-reference-forms\form_reporting_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC4801F8-F784-411D-BF2F-0CA04CF68182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA97D32-F5F1-4904-9AE2-BB2B6C35EBAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="wX8sA2MiVV4hem5/4RTiTmcDJYFB86HqbOVJt9hNWIZw6gEt8u041CW+Lo33VdE+XPx62lk39pDAbSFn1bENfA==" workbookSaltValue="4+KZsXogYyQ9Ht7v5WkMIg==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
   <si>
     <t>Name</t>
   </si>
@@ -123,9 +123,6 @@
     <t>Finalisation date</t>
   </si>
   <si>
-    <t>Fishery</t>
-  </si>
-  <si>
     <t>1.0.0</t>
   </si>
   <si>
@@ -148,6 +145,12 @@
   </si>
   <si>
     <t>Liaison officer</t>
+  </si>
+  <si>
+    <t>Vessel type</t>
+  </si>
+  <si>
+    <t>Configuration</t>
   </si>
 </sst>
 </file>
@@ -1209,7 +1212,7 @@
     <row r="1" spans="2:8" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="68" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="69"/>
       <c r="D2" s="69"/>
@@ -1233,14 +1236,14 @@
         <v>9</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E4" s="16"/>
       <c r="F4" s="14" t="s">
         <v>7</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H4" s="18"/>
     </row>
@@ -1276,7 +1279,7 @@
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="19"/>
       <c r="C8" s="67" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D8" s="67"/>
       <c r="E8" s="20"/>
@@ -1406,7 +1409,7 @@
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="19"/>
       <c r="C20" s="41" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="20"/>
@@ -1516,7 +1519,7 @@
     <col min="5" max="5" width="11.42578125" style="39" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" style="38" customWidth="1"/>
     <col min="7" max="7" width="11.42578125" style="45" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="38"/>
+    <col min="8" max="8" width="15.7109375" style="38" customWidth="1"/>
     <col min="9" max="9" width="14.28515625" style="39" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.140625" style="38" customWidth="1"/>
     <col min="11" max="11" width="12.140625" style="39" customWidth="1"/>
@@ -1544,7 +1547,7 @@
     </row>
     <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="68" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="69"/>
       <c r="D2" s="69"/>
@@ -1580,7 +1583,7 @@
     <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="62" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="74" t="s">
         <v>12</v>
@@ -1610,7 +1613,7 @@
     </row>
     <row r="5" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="55" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C5" s="61" t="s">
         <v>8</v>
@@ -1628,7 +1631,7 @@
         <v>23</v>
       </c>
       <c r="H5" s="55" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="I5" s="56" t="s">
         <v>15</v>
@@ -1637,7 +1640,7 @@
         <v>16</v>
       </c>
       <c r="K5" s="56" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L5" s="55" t="s">
         <v>8</v>
@@ -2306,7 +2309,7 @@
       <c r="L55" s="36"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="4/x7C4c4a0AVjOBj6btm9hOkWI9rn64Xb2MGYaWzP1gOCmRzIyayQx4ap4mNv9s4uluXIm2VuMoUCNU9Zv82wg==" saltValue="9FPR1JcRdNMeuwdMyreDEw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="kiQTEPL4oEo/2qZDsNw9GXsxKzjVlPg4a6Nc1pevXYFCxYI5O1RW1QMnQ7wJl2NCmbJbsu9xC5UCAm9KWirCqQ==" saltValue="4e6mAyh86NxjRxNgc0n2pw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="6">
     <mergeCell ref="B2:O3"/>
     <mergeCell ref="C4:E4"/>
@@ -2320,8 +2323,11 @@
       <formula>B6=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:L5 B5:F5" xr:uid="{62AC337C-43B8-43CC-ABCC-7EE87C42A16F}">
+  <dataValidations count="2">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:F5 I5:L5 H5" xr:uid="{62AC337C-43B8-43CC-ABCC-7EE87C42A16F}">
+      <formula1>"&lt;0&gt;0"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{5B262113-95A2-485C-B5B5-1EDF93672530}">
       <formula1>"&lt;0&gt;0"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2330,12 +2336,12 @@
     <hyperlink ref="D5" r:id="rId2" location="sourcesFC" xr:uid="{D508B0C5-71F1-4418-BA5D-6D532A3A0D47}"/>
     <hyperlink ref="E5" r:id="rId3" location="processingsFC" xr:uid="{3B28F9E8-FD32-4256-82C2-97BF03FEE964}"/>
     <hyperlink ref="F5" r:id="rId4" location="coverageTypes" xr:uid="{15A256B6-6B98-4ABF-81CC-D96AC29A08E2}"/>
-    <hyperlink ref="H5" r:id="rId5" location="boatTypes" xr:uid="{DADB17F2-537E-4DBC-AFEA-6EE304F8C6D0}"/>
+    <hyperlink ref="H5" r:id="rId5" location="boatTypes" display="Type" xr:uid="{DADB17F2-537E-4DBC-AFEA-6EE304F8C6D0}"/>
     <hyperlink ref="I5" r:id="rId6" location="mechanizationTypes" xr:uid="{40C3FFA1-CD46-4638-8E84-B19E43E165D4}"/>
     <hyperlink ref="J5" r:id="rId7" location="fishPreservationMethods" xr:uid="{2A56DBD0-E939-42A6-98DA-87DA852FD2E9}"/>
     <hyperlink ref="K5" r:id="rId8" location="fishStorageTypes" xr:uid="{9C5A0F26-DE48-4B7A-BF87-82196056DE69}"/>
     <hyperlink ref="L5" r:id="rId9" location="boatClassTypes" xr:uid="{263265AE-A782-4C7E-A95B-56C7C8AA2144}"/>
-    <hyperlink ref="B5" r:id="rId10" location="fisheries" xr:uid="{9C9CCABD-E884-4981-9553-0A805CCD876C}"/>
+    <hyperlink ref="B5" r:id="rId10" location="Vessel_Types" xr:uid="{9938127B-C147-49BE-9C85-EBE93EF4251D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>

</xml_diff>